<commit_message>
1. Test Base moved from com.test to com.dev 2. Added Login and Logout to pageObject model
Signed-off-by: debasis <debasis.dash@hpe.com>
</commit_message>
<xml_diff>
--- a/src/main/resources/Test-result/testout.xlsx
+++ b/src/main/resources/Test-result/testout.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="52">
   <si>
     <t>Testcase id</t>
   </si>
@@ -167,6 +167,9 @@
   </si>
   <si>
     <t>C:\Users\dashd\workspace\com.dsp.test/src/main/resources/Test-result/screenshots/createPackage_19_11_2017_09_37_57.png</t>
+  </si>
+  <si>
+    <t>C:\Users\dashd\workspace\com.dsp.test/src/main/resources/Test-result/screenshots/createPackage_20_11_2017_06_19_52.png</t>
   </si>
 </sst>
 </file>
@@ -816,7 +819,7 @@
         <v>46</v>
       </c>
       <c r="K4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="L4" s="9" t="s">
         <v>23</v>

</xml_diff>